<commit_message>
Added code for Homepage and customer page
</commit_message>
<xml_diff>
--- a/LiveProject/src/com/liveutility/TestData.xlsx
+++ b/LiveProject/src/com/liveutility/TestData.xlsx
@@ -8,16 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="NewCustomer" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Username</t>
   </si>
@@ -59,19 +58,110 @@
   </si>
   <si>
     <t>Both correct</t>
+  </si>
+  <si>
+    <t>CustomerName</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>Harish</t>
+  </si>
+  <si>
+    <t>Thiruvananthapuram</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>abcd@gmail.com</t>
+  </si>
+  <si>
+    <t>Test#123</t>
+  </si>
+  <si>
+    <t>Pavithra</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Telungana</t>
+  </si>
+  <si>
+    <t>efgh@gmail.com</t>
+  </si>
+  <si>
+    <t>Test#456</t>
+  </si>
+  <si>
+    <t>Dormula</t>
+  </si>
+  <si>
+    <t>Madurai</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>krishnanmeena363@gmail.com</t>
+  </si>
+  <si>
+    <t>Test#789</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Swami Vivekananda Lane Karamana</t>
+  </si>
+  <si>
+    <t>Narayana Kandalu Vedhiranth</t>
+  </si>
+  <si>
+    <t>Alagar nagar Pudhur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,14 +196,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -512,12 +608,144 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2">
+        <v>695002</v>
+      </c>
+      <c r="G2">
+        <v>9851478957</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3">
+        <v>500004</v>
+      </c>
+      <c r="G3">
+        <v>9851478000</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4">
+        <v>590684</v>
+      </c>
+      <c r="G4">
+        <v>9851478123</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>